<commit_message>
Corrected typos in TP4 data
</commit_message>
<xml_diff>
--- a/metadata/E5_QC.xlsx
+++ b/metadata/E5_QC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/timeseries/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC43A285-1B57-AB49-94E6-0A79158E5A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C31FC447-BFAC-5647-A867-59C03295916D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38400" yWindow="-1940" windowWidth="22860" windowHeight="19760" activeTab="4" xr2:uid="{9DA2C447-80F7-4347-8868-AE0AC17FBA84}"/>
+    <workbookView xWindow="-37380" yWindow="-2080" windowWidth="22860" windowHeight="19760" activeTab="3" xr2:uid="{9DA2C447-80F7-4347-8868-AE0AC17FBA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Color key" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="205">
   <si>
     <t>ANSWER</t>
   </si>
@@ -642,6 +642,18 @@
   <si>
     <t>Now POR-296 ; has been referred to as POR_385 before and is same coral; POR-387 is in mystery, relabel these in data as POR-385; resolved</t>
   </si>
+  <si>
+    <t xml:space="preserve">ACR-256 and ACR-267 bags "swapped" in notebook? </t>
+  </si>
+  <si>
+    <t>There is a POR-85 in the data, typo, in notebook. Resolved</t>
+  </si>
+  <si>
+    <t>In notebook as plate 2 was a typo as "PCO" rather than "POC"; resolved</t>
+  </si>
+  <si>
+    <t>Not sampled for protein</t>
+  </si>
 </sst>
 </file>
 
@@ -10256,9 +10268,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E77009AC-EDAD-2244-A553-6617E39CB99E}">
   <dimension ref="A1:N141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L93" sqref="L93"/>
+      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -10267,6 +10279,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="12" t="s">
+        <v>165</v>
+      </c>
       <c r="B1" t="s">
         <v>184</v>
       </c>
@@ -13394,7 +13409,7 @@
       <c r="A88">
         <v>50</v>
       </c>
-      <c r="B88" s="9" t="s">
+      <c r="B88" s="2" t="s">
         <v>66</v>
       </c>
       <c r="C88" t="b">
@@ -13415,7 +13430,7 @@
       <c r="H88" t="b">
         <v>1</v>
       </c>
-      <c r="I88" s="9" t="b">
+      <c r="I88" s="2" t="b">
         <v>0</v>
       </c>
       <c r="J88" t="b">
@@ -15328,9 +15343,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4259132-52BB-2B40-86FD-2A50319D60A8}">
   <dimension ref="A1:L145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E40" sqref="E40"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15976,6 +15991,9 @@
       <c r="K18" t="b">
         <v>1</v>
       </c>
+      <c r="L18" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -16160,6 +16178,9 @@
       <c r="K23" t="b">
         <v>1</v>
       </c>
+      <c r="L23" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24">
@@ -16341,8 +16362,11 @@
       <c r="J28" t="b">
         <v>1</v>
       </c>
-      <c r="K28" s="9" t="b">
-        <v>0</v>
+      <c r="K28" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="L28" t="s">
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -18222,7 +18246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -18257,7 +18281,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -18292,7 +18316,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -18327,11 +18351,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
-      <c r="B84" s="9" t="s">
+      <c r="B84" s="4" t="s">
         <v>91</v>
       </c>
       <c r="C84" t="b">
@@ -18358,11 +18382,14 @@
       <c r="J84" t="b">
         <v>1</v>
       </c>
-      <c r="K84" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K84" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L84" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -18397,7 +18424,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -18432,7 +18459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -18467,7 +18494,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -18502,7 +18529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -18537,7 +18564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -18572,7 +18599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -18607,7 +18634,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -18642,7 +18669,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -18677,7 +18704,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -18712,7 +18739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -18747,7 +18774,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -19215,7 +19242,7 @@
       <c r="A109">
         <v>108</v>
       </c>
-      <c r="B109" s="9" t="s">
+      <c r="B109" s="4" t="s">
         <v>114</v>
       </c>
       <c r="C109" t="b">
@@ -19242,8 +19269,11 @@
       <c r="J109" t="b">
         <v>1</v>
       </c>
-      <c r="K109" s="9" t="b">
-        <v>0</v>
+      <c r="K109" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="L109" t="s">
+        <v>202</v>
       </c>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated E5 QC sheet
</commit_message>
<xml_diff>
--- a/metadata/E5_QC.xlsx
+++ b/metadata/E5_QC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arianasnowhuffmyer/MyProjects/E5/timeseries/metadata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE75017-DC8C-544A-90F6-C520F051DE73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AC4152E-CF6F-9E4B-B215-2CE3E8C5BCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37380" yWindow="-2080" windowWidth="25040" windowHeight="19760" activeTab="4" xr2:uid="{9DA2C447-80F7-4347-8868-AE0AC17FBA84}"/>
+    <workbookView xWindow="-37580" yWindow="-2000" windowWidth="25040" windowHeight="19760" activeTab="4" xr2:uid="{9DA2C447-80F7-4347-8868-AE0AC17FBA84}"/>
   </bookViews>
   <sheets>
     <sheet name="Color key" sheetId="5" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="213">
   <si>
     <t>ANSWER</t>
   </si>
@@ -671,6 +671,12 @@
   </si>
   <si>
     <t>Typo - in notebook written as ACR-390, but entered in datasheet as ACR-364</t>
+  </si>
+  <si>
+    <t>CHECK ALL PLATEMAPS</t>
+  </si>
+  <si>
+    <t>PLATEMAPS DON’T MATCH NOTEBOOK</t>
   </si>
 </sst>
 </file>
@@ -759,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -773,6 +779,7 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10288,7 +10295,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="L34" sqref="L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15359,16 +15366,19 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4259132-52BB-2B40-86FD-2A50319D60A8}">
-  <dimension ref="A1:L145"/>
+  <dimension ref="A1:R145"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="10" max="10" width="10.83203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="B1" s="5" t="s">
         <v>9</v>
       </c>
@@ -15393,14 +15403,14 @@
       <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="5" t="s">
+      <c r="J1" s="13" t="s">
         <v>17</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -15428,7 +15438,7 @@
       <c r="I2" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J2" s="2" t="b">
+      <c r="J2" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K2" s="2" t="b">
@@ -15437,8 +15447,12 @@
       <c r="L2" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P2" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -15466,14 +15480,19 @@
       <c r="I3" t="b">
         <v>1</v>
       </c>
-      <c r="J3" s="9" t="b">
+      <c r="J3" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="P3" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -15501,14 +15520,14 @@
       <c r="I4" t="b">
         <v>1</v>
       </c>
-      <c r="J4" s="9" t="b">
+      <c r="J4" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -15536,14 +15555,14 @@
       <c r="I5" t="b">
         <v>1</v>
       </c>
-      <c r="J5" s="9" t="b">
+      <c r="J5" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K5" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -15571,7 +15590,7 @@
       <c r="I6" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J6" s="2" t="b">
+      <c r="J6" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K6" s="2" t="b">
@@ -15581,7 +15600,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -15609,14 +15628,14 @@
       <c r="I7" t="b">
         <v>1</v>
       </c>
-      <c r="J7" s="9" t="b">
+      <c r="J7" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K7" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -15644,14 +15663,14 @@
       <c r="I8" t="b">
         <v>1</v>
       </c>
-      <c r="J8" t="b">
+      <c r="J8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -15679,14 +15698,14 @@
       <c r="I9" t="b">
         <v>1</v>
       </c>
-      <c r="J9" t="b">
+      <c r="J9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -15714,7 +15733,7 @@
       <c r="I10" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J10" s="2" t="b">
+      <c r="J10" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K10" s="2" t="b">
@@ -15724,7 +15743,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -15752,14 +15771,14 @@
       <c r="I11" t="b">
         <v>1</v>
       </c>
-      <c r="J11" t="b">
+      <c r="J11" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K11" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -15787,14 +15806,14 @@
       <c r="I12" t="b">
         <v>1</v>
       </c>
-      <c r="J12" t="b">
+      <c r="J12" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K12" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -15822,14 +15841,14 @@
       <c r="I13" t="b">
         <v>1</v>
       </c>
-      <c r="J13" t="b">
+      <c r="J13" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K13" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -15857,14 +15876,14 @@
       <c r="I14" t="b">
         <v>1</v>
       </c>
-      <c r="J14" t="b">
+      <c r="J14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K14" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -15892,7 +15911,7 @@
       <c r="I15" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J15" t="b">
+      <c r="J15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K15" s="9" t="b">
@@ -15902,7 +15921,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -15930,7 +15949,7 @@
       <c r="I16" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J16" t="b">
+      <c r="J16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K16" s="9" t="b">
@@ -15968,7 +15987,7 @@
       <c r="I17" t="b">
         <v>1</v>
       </c>
-      <c r="J17" t="b">
+      <c r="J17" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K17" t="b">
@@ -16003,7 +16022,7 @@
       <c r="I18" t="b">
         <v>1</v>
       </c>
-      <c r="J18" s="9" t="b">
+      <c r="J18" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K18" t="b">
@@ -16041,7 +16060,7 @@
       <c r="I19" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J19" s="9" t="b">
+      <c r="J19" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K19" t="b">
@@ -16079,7 +16098,7 @@
       <c r="I20" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J20" s="2" t="b">
+      <c r="J20" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K20" s="2" t="b">
@@ -16117,7 +16136,7 @@
       <c r="I21" t="b">
         <v>1</v>
       </c>
-      <c r="J21" t="b">
+      <c r="J21" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K21" t="b">
@@ -16152,7 +16171,7 @@
       <c r="I22" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J22" s="2" t="b">
+      <c r="J22" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K22" s="2" t="b">
@@ -16190,7 +16209,7 @@
       <c r="I23" t="b">
         <v>1</v>
       </c>
-      <c r="J23" s="9" t="b">
+      <c r="J23" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K23" t="b">
@@ -16228,7 +16247,7 @@
       <c r="I24" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J24" s="2" t="b">
+      <c r="J24" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K24" s="2" t="b">
@@ -16266,7 +16285,7 @@
       <c r="I25" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J25" t="b">
+      <c r="J25" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K25" s="9" t="b">
@@ -16304,7 +16323,7 @@
       <c r="I26" t="b">
         <v>1</v>
       </c>
-      <c r="J26" t="b">
+      <c r="J26" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K26" t="b">
@@ -16339,7 +16358,7 @@
       <c r="I27" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J27" s="2" t="b">
+      <c r="J27" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K27" s="2" t="b">
@@ -16377,7 +16396,7 @@
       <c r="I28" t="b">
         <v>1</v>
       </c>
-      <c r="J28" t="b">
+      <c r="J28" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K28" s="2" t="b">
@@ -16415,7 +16434,7 @@
       <c r="I29" t="b">
         <v>1</v>
       </c>
-      <c r="J29" t="b">
+      <c r="J29" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K29" t="b">
@@ -16450,7 +16469,7 @@
       <c r="I30" t="b">
         <v>1</v>
       </c>
-      <c r="J30" t="b">
+      <c r="J30" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K30" t="b">
@@ -16485,7 +16504,7 @@
       <c r="I31" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J31" s="2" t="b">
+      <c r="J31" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K31" s="2" t="b">
@@ -16523,7 +16542,7 @@
       <c r="I32" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J32" s="2" t="b">
+      <c r="J32" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K32" s="2" t="b">
@@ -16562,7 +16581,7 @@
         <v>1</v>
       </c>
       <c r="J33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K33" t="b">
         <v>1</v>
@@ -16599,7 +16618,7 @@
       <c r="I34" t="b">
         <v>1</v>
       </c>
-      <c r="J34" s="9" t="b">
+      <c r="J34" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K34" t="b">
@@ -16634,7 +16653,7 @@
       <c r="I35" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J35" s="2" t="b">
+      <c r="J35" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K35" s="2" t="b">
@@ -16672,7 +16691,7 @@
       <c r="I36" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J36" s="2" t="b">
+      <c r="J36" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K36" s="2" t="b">
@@ -16710,7 +16729,7 @@
       <c r="I37" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J37" s="2" t="b">
+      <c r="J37" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K37" s="2" t="b">
@@ -16786,7 +16805,7 @@
       <c r="I39" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J39" s="2" t="b">
+      <c r="J39" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K39" s="2" t="b">
@@ -16824,7 +16843,7 @@
       <c r="I40" t="b">
         <v>1</v>
       </c>
-      <c r="J40" s="9" t="b">
+      <c r="J40" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K40" t="b">
@@ -16862,7 +16881,7 @@
       <c r="I41" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J41" s="2" t="b">
+      <c r="J41" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K41" s="2" t="b">
@@ -16900,7 +16919,7 @@
       <c r="I42" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J42" s="2" t="b">
+      <c r="J42" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K42" s="2" t="b">
@@ -16938,7 +16957,7 @@
       <c r="I43" t="b">
         <v>1</v>
       </c>
-      <c r="J43" s="9" t="b">
+      <c r="J43" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K43" t="b">
@@ -16973,7 +16992,7 @@
       <c r="I44" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J44" s="2" t="b">
+      <c r="J44" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K44" s="2" t="b">
@@ -17011,7 +17030,7 @@
       <c r="I45" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J45" s="2" t="b">
+      <c r="J45" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K45" s="2" t="b">
@@ -17049,7 +17068,7 @@
       <c r="I46" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J46" s="2" t="b">
+      <c r="J46" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K46" s="2" t="b">
@@ -17087,7 +17106,7 @@
       <c r="I47" t="b">
         <v>1</v>
       </c>
-      <c r="J47" t="b">
+      <c r="J47" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K47" t="b">
@@ -17122,7 +17141,7 @@
       <c r="I48" t="b">
         <v>1</v>
       </c>
-      <c r="J48" s="9" t="b">
+      <c r="J48" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K48" t="b">
@@ -17157,7 +17176,7 @@
       <c r="I49" t="b">
         <v>1</v>
       </c>
-      <c r="J49" t="b">
+      <c r="J49" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K49" t="b">
@@ -17192,7 +17211,7 @@
       <c r="I50" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J50" s="2" t="b">
+      <c r="J50" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K50" s="2" t="b">
@@ -17230,7 +17249,7 @@
       <c r="I51" t="b">
         <v>1</v>
       </c>
-      <c r="J51" t="b">
+      <c r="J51" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K51" t="b">
@@ -17265,7 +17284,7 @@
       <c r="I52" t="b">
         <v>1</v>
       </c>
-      <c r="J52" t="b">
+      <c r="J52" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K52" t="b">
@@ -17300,7 +17319,7 @@
       <c r="I53" t="b">
         <v>1</v>
       </c>
-      <c r="J53" t="b">
+      <c r="J53" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K53" t="b">
@@ -17335,7 +17354,7 @@
       <c r="I54" t="b">
         <v>1</v>
       </c>
-      <c r="J54" t="b">
+      <c r="J54" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K54" t="b">
@@ -17370,7 +17389,7 @@
       <c r="I55" t="b">
         <v>1</v>
       </c>
-      <c r="J55" t="b">
+      <c r="J55" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K55" t="b">
@@ -17405,7 +17424,7 @@
       <c r="I56" t="b">
         <v>1</v>
       </c>
-      <c r="J56" t="b">
+      <c r="J56" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K56" t="b">
@@ -17440,7 +17459,7 @@
       <c r="I57" t="b">
         <v>1</v>
       </c>
-      <c r="J57" s="9" t="b">
+      <c r="J57" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K57" t="b">
@@ -17475,7 +17494,7 @@
       <c r="I58" t="b">
         <v>1</v>
       </c>
-      <c r="J58" t="b">
+      <c r="J58" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K58" t="b">
@@ -17510,7 +17529,7 @@
       <c r="I59" t="b">
         <v>1</v>
       </c>
-      <c r="J59" t="b">
+      <c r="J59" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K59" t="b">
@@ -17545,7 +17564,7 @@
       <c r="I60" t="b">
         <v>1</v>
       </c>
-      <c r="J60" t="b">
+      <c r="J60" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K60" t="b">
@@ -17580,7 +17599,7 @@
       <c r="I61" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J61" s="2" t="b">
+      <c r="J61" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K61" s="2" t="b">
@@ -17618,7 +17637,7 @@
       <c r="I62" t="b">
         <v>1</v>
       </c>
-      <c r="J62" t="b">
+      <c r="J62" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K62" t="b">
@@ -17653,7 +17672,7 @@
       <c r="I63" t="b">
         <v>1</v>
       </c>
-      <c r="J63" t="b">
+      <c r="J63" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K63" t="b">
@@ -17688,7 +17707,7 @@
       <c r="I64" t="b">
         <v>1</v>
       </c>
-      <c r="J64" t="b">
+      <c r="J64" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K64" t="b">
@@ -17723,7 +17742,7 @@
       <c r="I65" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J65" t="b">
+      <c r="J65" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K65" s="9" t="b">
@@ -17761,7 +17780,7 @@
       <c r="I66" t="b">
         <v>1</v>
       </c>
-      <c r="J66" t="b">
+      <c r="J66" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K66" t="b">
@@ -17796,7 +17815,7 @@
       <c r="I67" t="b">
         <v>1</v>
       </c>
-      <c r="J67" t="b">
+      <c r="J67" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K67" t="b">
@@ -17831,7 +17850,7 @@
       <c r="I68" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J68" s="2" t="b">
+      <c r="J68" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K68" s="2" t="b">
@@ -17869,7 +17888,7 @@
       <c r="I69" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J69" s="2" t="b">
+      <c r="J69" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K69" s="2" t="b">
@@ -17907,7 +17926,7 @@
       <c r="I70" t="b">
         <v>1</v>
       </c>
-      <c r="J70" t="b">
+      <c r="J70" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K70" t="b">
@@ -17942,7 +17961,7 @@
       <c r="I71" t="b">
         <v>1</v>
       </c>
-      <c r="J71" t="b">
+      <c r="J71" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K71" t="b">
@@ -17977,7 +17996,7 @@
       <c r="I72" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J72" s="9" t="b">
+      <c r="J72" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K72" s="9" t="b">
@@ -18015,7 +18034,7 @@
       <c r="I73" t="b">
         <v>1</v>
       </c>
-      <c r="J73" t="b">
+      <c r="J73" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K73" t="b">
@@ -18050,7 +18069,7 @@
       <c r="I74" t="b">
         <v>1</v>
       </c>
-      <c r="J74" t="b">
+      <c r="J74" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K74" t="b">
@@ -18085,7 +18104,7 @@
       <c r="I75" t="b">
         <v>1</v>
       </c>
-      <c r="J75" t="b">
+      <c r="J75" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K75" t="b">
@@ -18120,7 +18139,7 @@
       <c r="I76" t="b">
         <v>1</v>
       </c>
-      <c r="J76" t="b">
+      <c r="J76" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K76" t="b">
@@ -18155,7 +18174,7 @@
       <c r="I77" t="b">
         <v>1</v>
       </c>
-      <c r="J77" t="b">
+      <c r="J77" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K77" t="b">
@@ -18190,7 +18209,7 @@
       <c r="I78" t="b">
         <v>1</v>
       </c>
-      <c r="J78" t="b">
+      <c r="J78" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K78" t="b">
@@ -18225,7 +18244,7 @@
       <c r="I79" t="b">
         <v>1</v>
       </c>
-      <c r="J79" t="b">
+      <c r="J79" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K79" t="b">
@@ -18260,7 +18279,7 @@
       <c r="I80" t="b">
         <v>1</v>
       </c>
-      <c r="J80" s="9" t="b">
+      <c r="J80" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K80" t="b">
@@ -18295,7 +18314,7 @@
       <c r="I81" t="b">
         <v>1</v>
       </c>
-      <c r="J81" t="b">
+      <c r="J81" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K81" t="b">
@@ -18330,7 +18349,7 @@
       <c r="I82" t="b">
         <v>1</v>
       </c>
-      <c r="J82" t="b">
+      <c r="J82" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K82" t="b">
@@ -18365,7 +18384,7 @@
       <c r="I83" t="b">
         <v>1</v>
       </c>
-      <c r="J83" t="b">
+      <c r="J83" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K83" t="b">
@@ -18400,7 +18419,7 @@
       <c r="I84" t="b">
         <v>1</v>
       </c>
-      <c r="J84" t="b">
+      <c r="J84" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K84" s="4" t="b">
@@ -18438,7 +18457,7 @@
       <c r="I85" t="b">
         <v>1</v>
       </c>
-      <c r="J85" t="b">
+      <c r="J85" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K85" t="b">
@@ -18473,7 +18492,7 @@
       <c r="I86" t="b">
         <v>1</v>
       </c>
-      <c r="J86" t="b">
+      <c r="J86" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K86" t="b">
@@ -18508,7 +18527,7 @@
       <c r="I87" t="b">
         <v>1</v>
       </c>
-      <c r="J87" t="b">
+      <c r="J87" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K87" t="b">
@@ -18543,7 +18562,7 @@
       <c r="I88" t="b">
         <v>1</v>
       </c>
-      <c r="J88" t="b">
+      <c r="J88" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K88" t="b">
@@ -18578,7 +18597,7 @@
       <c r="I89" t="b">
         <v>1</v>
       </c>
-      <c r="J89" t="b">
+      <c r="J89" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K89" t="b">
@@ -18613,7 +18632,7 @@
       <c r="I90" t="b">
         <v>1</v>
       </c>
-      <c r="J90" t="b">
+      <c r="J90" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K90" t="b">
@@ -18651,7 +18670,7 @@
       <c r="I91" t="b">
         <v>1</v>
       </c>
-      <c r="J91" t="b">
+      <c r="J91" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K91" t="b">
@@ -18686,7 +18705,7 @@
       <c r="I92" t="b">
         <v>1</v>
       </c>
-      <c r="J92" t="b">
+      <c r="J92" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K92" t="b">
@@ -18721,7 +18740,7 @@
       <c r="I93" t="b">
         <v>1</v>
       </c>
-      <c r="J93" s="9" t="b">
+      <c r="J93" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K93" t="b">
@@ -18756,7 +18775,7 @@
       <c r="I94" t="b">
         <v>1</v>
       </c>
-      <c r="J94" t="b">
+      <c r="J94" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K94" t="b">
@@ -18791,7 +18810,7 @@
       <c r="I95" t="b">
         <v>1</v>
       </c>
-      <c r="J95" t="b">
+      <c r="J95" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K95" t="b">
@@ -18826,7 +18845,7 @@
       <c r="I96" t="b">
         <v>1</v>
       </c>
-      <c r="J96" t="b">
+      <c r="J96" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K96" t="b">
@@ -18861,7 +18880,7 @@
       <c r="I97" t="b">
         <v>1</v>
       </c>
-      <c r="J97" t="b">
+      <c r="J97" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K97" t="b">
@@ -18896,7 +18915,7 @@
       <c r="I98" t="b">
         <v>1</v>
       </c>
-      <c r="J98" t="b">
+      <c r="J98" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K98" t="b">
@@ -18931,7 +18950,7 @@
       <c r="I99" t="b">
         <v>1</v>
       </c>
-      <c r="J99" t="b">
+      <c r="J99" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K99" t="b">
@@ -18966,7 +18985,7 @@
       <c r="I100" t="b">
         <v>1</v>
       </c>
-      <c r="J100" t="b">
+      <c r="J100" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K100" t="b">
@@ -19001,7 +19020,7 @@
       <c r="I101" t="b">
         <v>1</v>
       </c>
-      <c r="J101" t="b">
+      <c r="J101" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K101" t="b">
@@ -19036,7 +19055,7 @@
       <c r="I102" t="b">
         <v>1</v>
       </c>
-      <c r="J102" t="b">
+      <c r="J102" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K102" t="b">
@@ -19074,7 +19093,7 @@
       <c r="I103" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J103" s="2" t="b">
+      <c r="J103" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K103" s="2" t="b">
@@ -19112,7 +19131,7 @@
       <c r="I104" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J104" s="2" t="b">
+      <c r="J104" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K104" s="2" t="b">
@@ -19150,7 +19169,7 @@
       <c r="I105" t="b">
         <v>1</v>
       </c>
-      <c r="J105" t="b">
+      <c r="J105" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K105" t="b">
@@ -19185,7 +19204,7 @@
       <c r="I106" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J106" t="b">
+      <c r="J106" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K106" s="9" t="b">
@@ -19223,7 +19242,7 @@
       <c r="I107" t="b">
         <v>1</v>
       </c>
-      <c r="J107" t="b">
+      <c r="J107" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K107" t="b">
@@ -19258,7 +19277,7 @@
       <c r="I108" t="b">
         <v>1</v>
       </c>
-      <c r="J108" t="b">
+      <c r="J108" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K108" t="b">
@@ -19293,7 +19312,7 @@
       <c r="I109" t="b">
         <v>1</v>
       </c>
-      <c r="J109" t="b">
+      <c r="J109" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K109" s="4" t="b">
@@ -19331,7 +19350,7 @@
       <c r="I110" t="b">
         <v>1</v>
       </c>
-      <c r="J110" t="b">
+      <c r="J110" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K110" t="b">
@@ -19366,7 +19385,7 @@
       <c r="I111" t="b">
         <v>1</v>
       </c>
-      <c r="J111" t="b">
+      <c r="J111" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K111" t="b">
@@ -19401,7 +19420,7 @@
       <c r="I112" t="b">
         <v>1</v>
       </c>
-      <c r="J112" t="b">
+      <c r="J112" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K112" t="b">
@@ -19436,7 +19455,7 @@
       <c r="I113" t="b">
         <v>1</v>
       </c>
-      <c r="J113" t="b">
+      <c r="J113" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K113" t="b">
@@ -19471,7 +19490,7 @@
       <c r="I114" t="b">
         <v>1</v>
       </c>
-      <c r="J114" t="b">
+      <c r="J114" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K114" t="b">
@@ -19506,7 +19525,7 @@
       <c r="I115" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J115" s="2" t="b">
+      <c r="J115" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K115" s="2" t="b">
@@ -19544,7 +19563,7 @@
       <c r="I116" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J116" s="2" t="b">
+      <c r="J116" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K116" s="2" t="b">
@@ -19582,7 +19601,7 @@
       <c r="I117" t="b">
         <v>1</v>
       </c>
-      <c r="J117" t="b">
+      <c r="J117" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K117" t="b">
@@ -19617,7 +19636,7 @@
       <c r="I118" t="b">
         <v>1</v>
       </c>
-      <c r="J118" t="b">
+      <c r="J118" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K118" t="b">
@@ -19655,7 +19674,7 @@
       <c r="I119" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="J119" t="b">
+      <c r="J119" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K119" t="b">
@@ -19693,7 +19712,7 @@
       <c r="I120" t="b">
         <v>1</v>
       </c>
-      <c r="J120" t="b">
+      <c r="J120" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K120" t="b">
@@ -19728,7 +19747,7 @@
       <c r="I121" t="b">
         <v>1</v>
       </c>
-      <c r="J121" t="b">
+      <c r="J121" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K121" t="b">
@@ -19763,7 +19782,7 @@
       <c r="I122" t="b">
         <v>1</v>
       </c>
-      <c r="J122" t="b">
+      <c r="J122" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K122" t="b">
@@ -19798,7 +19817,7 @@
       <c r="I123" t="b">
         <v>1</v>
       </c>
-      <c r="J123" t="b">
+      <c r="J123" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K123" t="b">
@@ -19833,7 +19852,7 @@
       <c r="I124" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J124" s="2" t="b">
+      <c r="J124" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K124" s="2" t="b">
@@ -19871,7 +19890,7 @@
       <c r="I125" t="b">
         <v>1</v>
       </c>
-      <c r="J125" t="b">
+      <c r="J125" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K125" t="b">
@@ -19906,7 +19925,7 @@
       <c r="I126" t="b">
         <v>1</v>
       </c>
-      <c r="J126" t="b">
+      <c r="J126" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K126" t="b">
@@ -19941,7 +19960,7 @@
       <c r="I127" t="b">
         <v>1</v>
       </c>
-      <c r="J127" t="b">
+      <c r="J127" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K127" t="b">
@@ -19976,7 +19995,7 @@
       <c r="I128" t="b">
         <v>1</v>
       </c>
-      <c r="J128" t="b">
+      <c r="J128" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K128" t="b">
@@ -20011,7 +20030,7 @@
       <c r="I129" t="b">
         <v>1</v>
       </c>
-      <c r="J129" t="b">
+      <c r="J129" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K129" t="b">
@@ -20046,7 +20065,7 @@
       <c r="I130" t="b">
         <v>1</v>
       </c>
-      <c r="J130" t="b">
+      <c r="J130" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K130" t="b">
@@ -20081,7 +20100,7 @@
       <c r="I131" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J131" s="9" t="b">
+      <c r="J131" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K131" s="2" t="b">
@@ -20119,7 +20138,7 @@
       <c r="I132" t="b">
         <v>1</v>
       </c>
-      <c r="J132" t="b">
+      <c r="J132" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K132" t="b">
@@ -20154,7 +20173,7 @@
       <c r="I133" t="b">
         <v>1</v>
       </c>
-      <c r="J133" t="b">
+      <c r="J133" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K133" t="b">
@@ -20189,7 +20208,7 @@
       <c r="I134" t="b">
         <v>1</v>
       </c>
-      <c r="J134" t="b">
+      <c r="J134" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K134" t="b">
@@ -20227,7 +20246,7 @@
       <c r="I135" t="b">
         <v>1</v>
       </c>
-      <c r="J135" t="b">
+      <c r="J135" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K135" t="b">
@@ -20262,7 +20281,7 @@
       <c r="I136" t="b">
         <v>1</v>
       </c>
-      <c r="J136" t="b">
+      <c r="J136" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K136" t="b">
@@ -20297,7 +20316,7 @@
       <c r="I137" t="b">
         <v>1</v>
       </c>
-      <c r="J137" t="b">
+      <c r="J137" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K137" t="b">
@@ -20332,7 +20351,7 @@
       <c r="I138" t="b">
         <v>1</v>
       </c>
-      <c r="J138" t="b">
+      <c r="J138" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K138" t="b">
@@ -20367,7 +20386,7 @@
       <c r="I139" s="4" t="b">
         <v>1</v>
       </c>
-      <c r="J139" s="4" t="b">
+      <c r="J139" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K139" s="4" t="b">
@@ -20405,7 +20424,7 @@
       <c r="I140" t="b">
         <v>1</v>
       </c>
-      <c r="J140" t="b">
+      <c r="J140" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K140" t="b">
@@ -20440,7 +20459,7 @@
       <c r="I141" t="b">
         <v>1</v>
       </c>
-      <c r="J141" t="b">
+      <c r="J141" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K141" t="b">
@@ -20475,7 +20494,7 @@
       <c r="I142" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="J142" t="b">
+      <c r="J142" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K142" t="b">
@@ -20513,7 +20532,7 @@
       <c r="I143" t="b">
         <v>1</v>
       </c>
-      <c r="J143" t="b">
+      <c r="J143" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K143" t="b">
@@ -20548,7 +20567,7 @@
       <c r="I144" t="b">
         <v>1</v>
       </c>
-      <c r="J144" t="b">
+      <c r="J144" s="1" t="b">
         <v>1</v>
       </c>
       <c r="K144" t="b">
@@ -20583,7 +20602,7 @@
       <c r="I145" s="2" t="b">
         <v>0</v>
       </c>
-      <c r="J145" s="2" t="b">
+      <c r="J145" s="1" t="b">
         <v>0</v>
       </c>
       <c r="K145" s="2" t="b">

</xml_diff>